<commit_message>
Added first draft of the PowerBI project reports
</commit_message>
<xml_diff>
--- a/Dimension Tables/Congestion Surchage.xlsx
+++ b/Dimension Tables/Congestion Surchage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\PowerBI Projects\Trips Project\NYC-Trips-Project\Dimension Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA83AB98-6C8E-45C9-8116-13303159CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808184C-B425-4666-8AC2-225310B12DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F7AF5E2-2D94-4C69-A6E2-0D39240E5C09}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{7F7AF5E2-2D94-4C69-A6E2-0D39240E5C09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,6 +97,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25801FCD-9B4A-42D2-8B12-0A33721913A7}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{25801FCD-9B4A-42D2-8B12-0A33721913A7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B9ADD554-2871-4A25-8512-33ED1208D461}" name="Code"/>
+    <tableColumn id="2" xr3:uid="{DCE25D84-3DB8-48DA-9D46-DBA856BFF5F9}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,12 +430,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -445,5 +456,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>